<commit_message>
unit tests fixed for CI (needed to use the env var again since CI loads files differently (this group_unit_test passes locally!)
</commit_message>
<xml_diff>
--- a/tests/test_data/utils/Correct Universal 3D CoordStand Table.xlsx
+++ b/tests/test_data/utils/Correct Universal 3D CoordStand Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahan/sciebo/PythonCode/gaita_repo/tests/test_data/utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E4B502-BB97-A343-B14B-DBF4A1B79417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2FB93E-D561-FA46-996B-7783E67D3487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34360" yWindow="4100" windowWidth="28040" windowHeight="17440" xr2:uid="{B64B93B7-5589-E74D-9F24-A2104D993A81}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{B64B93B7-5589-E74D-9F24-A2104D993A81}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -441,7 +441,7 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="1">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>